<commit_message>
Update seed in xlsx file
</commit_message>
<xml_diff>
--- a/db/Kilogram_seed.xlsx
+++ b/db/Kilogram_seed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonyjhuang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonyjhuang/Desktop/Kilogram/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A985DD7-4E6D-4C4F-AB28-5825BCCA72ED}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8528996-7655-0342-8AB4-8A0B75089798}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="4" xr2:uid="{CE421DB2-E124-D246-ADE4-A8496529D3A8}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Likes!$A$1:$A$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Posts!$C$2:$AC$29</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="105">
   <si>
     <t>Follow.create!({</t>
   </si>
@@ -2390,11 +2390,11 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1">
         <f ca="1">RANDBETWEEN(1,28)</f>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1">
         <v>18</v>
@@ -2406,7 +2406,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A60" ca="1" si="0">RANDBETWEEN(1,28)</f>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B60" ca="1" si="1">RANDBETWEEN(1,5)</f>
@@ -2422,11 +2422,11 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2438,7 +2438,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
@@ -2454,11 +2454,11 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -2470,11 +2470,11 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>11</v>
@@ -2486,11 +2486,11 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>18</v>
@@ -2502,7 +2502,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
@@ -2518,11 +2518,11 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -2534,7 +2534,7 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
@@ -2550,11 +2550,11 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>28</v>
@@ -2566,11 +2566,11 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>24</v>
@@ -2582,11 +2582,11 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -2598,7 +2598,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
@@ -2614,7 +2614,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
@@ -2630,11 +2630,11 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -2646,11 +2646,11 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17">
         <v>16</v>
@@ -2662,11 +2662,11 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <v>25</v>
@@ -2678,11 +2678,11 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <v>8</v>
@@ -2694,11 +2694,11 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -2710,11 +2710,11 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>24</v>
@@ -2726,11 +2726,11 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>27</v>
@@ -2742,11 +2742,11 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <v>13</v>
@@ -2758,11 +2758,11 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>26</v>
@@ -2774,11 +2774,11 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25">
         <v>18</v>
@@ -2790,7 +2790,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
@@ -2806,7 +2806,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
@@ -2822,11 +2822,11 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>14</v>
@@ -2838,11 +2838,11 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -2854,11 +2854,11 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>7</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E31">
         <v>21</v>
@@ -2886,11 +2886,11 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -2902,11 +2902,11 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E33">
         <v>28</v>
@@ -2918,11 +2918,11 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E34">
         <v>23</v>
@@ -2934,11 +2934,11 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>14</v>
@@ -2950,11 +2950,11 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36">
         <v>27</v>
@@ -2966,11 +2966,11 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <v>19</v>
@@ -2982,11 +2982,11 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>15</v>
@@ -2998,11 +2998,11 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E39">
         <v>18</v>
@@ -3014,11 +3014,11 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>20</v>
@@ -3030,7 +3030,7 @@
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
@@ -3046,11 +3046,11 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E42">
         <v>23</v>
@@ -3062,7 +3062,7 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
@@ -3078,11 +3078,11 @@
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -3094,7 +3094,7 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
@@ -3110,11 +3110,11 @@
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E46">
         <v>24</v>
@@ -3126,11 +3126,11 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>19</v>
@@ -3142,11 +3142,11 @@
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E48">
         <v>12</v>
@@ -3158,17 +3158,17 @@
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
@@ -3178,27 +3178,27 @@
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
@@ -3208,57 +3208,57 @@
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
@@ -3268,11 +3268,11 @@
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3285,7 +3285,7 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3310,8 +3310,8 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>90</v>
+        <f t="shared" ref="A2:A29" ca="1" si="0">RANDBETWEEN(1,100)</f>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3323,7 +3323,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="str">
-        <f>C2&amp;"_"&amp;D2&amp;".jpeg"</f>
+        <f t="shared" ref="E2:E29" si="1">C2&amp;"_"&amp;D2&amp;".jpeg"</f>
         <v>1_6.jpeg</v>
       </c>
       <c r="F2" t="s">
@@ -3333,7 +3333,7 @@
         <v>22</v>
       </c>
       <c r="H2">
-        <f>C2</f>
+        <f t="shared" ref="H2:H29" si="2">C2</f>
         <v>1</v>
       </c>
       <c r="I2" t="s">
@@ -3343,7 +3343,7 @@
         <v>52</v>
       </c>
       <c r="K2" t="str">
-        <f>F2</f>
+        <f t="shared" ref="K2:K29" si="3">F2</f>
         <v>Portland Light House</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -3353,7 +3353,7 @@
         <v>63</v>
       </c>
       <c r="N2" t="str">
-        <f>G2</f>
+        <f t="shared" ref="N2:N29" si="4">G2</f>
         <v>Portland. ME</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -3363,7 +3363,7 @@
         <v>64</v>
       </c>
       <c r="Q2">
-        <f>H2</f>
+        <f t="shared" ref="Q2:Q29" si="5">H2</f>
         <v>1</v>
       </c>
       <c r="R2" t="s">
@@ -3373,7 +3373,7 @@
         <v>55</v>
       </c>
       <c r="U2" t="str">
-        <f>E2</f>
+        <f t="shared" ref="U2:U29" si="6">E2</f>
         <v>1_6.jpeg</v>
       </c>
       <c r="V2" s="3" t="s">
@@ -3383,7 +3383,7 @@
         <v>56</v>
       </c>
       <c r="X2" t="str">
-        <f>E2</f>
+        <f t="shared" ref="X2:X29" si="7">E2</f>
         <v>1_6.jpeg</v>
       </c>
       <c r="Y2" s="3" t="s">
@@ -3393,14 +3393,14 @@
         <v>60</v>
       </c>
       <c r="AC2" t="str">
-        <f>I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2&amp;S2&amp;T2&amp;U2&amp;V2&amp;W2&amp;X2&amp;Y2&amp;Z2&amp;AA2</f>
+        <f t="shared" ref="AC2:AC29" si="8">I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2&amp;S2&amp;T2&amp;U2&amp;V2&amp;W2&amp;X2&amp;Y2&amp;Z2&amp;AA2</f>
         <v>a = Post.new({caption: 'Portland Light House', location: 'Portland. ME', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_6.jpeg'), filename: '1_6.jpeg')a.save!</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>8</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -3412,7 +3412,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="str">
-        <f>C3&amp;"_"&amp;D3&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_11.jpeg</v>
       </c>
       <c r="F3" t="s">
@@ -3422,7 +3422,7 @@
         <v>68</v>
       </c>
       <c r="H3">
-        <f>C3</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I3" t="s">
@@ -3432,27 +3432,18 @@
         <v>52</v>
       </c>
       <c r="K3" t="str">
-        <f>F3</f>
+        <f t="shared" si="3"/>
         <v>Boomer staring into the flames</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" t="str">
-        <f>G3</f>
-        <v>'</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="O3" s="3"/>
       <c r="P3" t="s">
         <v>64</v>
       </c>
       <c r="Q3">
-        <f>H3</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R3" t="s">
@@ -3462,7 +3453,7 @@
         <v>55</v>
       </c>
       <c r="U3" t="str">
-        <f>E3</f>
+        <f t="shared" si="6"/>
         <v>1_11.jpeg</v>
       </c>
       <c r="V3" s="3" t="s">
@@ -3472,7 +3463,7 @@
         <v>56</v>
       </c>
       <c r="X3" t="str">
-        <f>E3</f>
+        <f t="shared" si="7"/>
         <v>1_11.jpeg</v>
       </c>
       <c r="Y3" s="3" t="s">
@@ -3482,14 +3473,14 @@
         <v>60</v>
       </c>
       <c r="AC3" t="str">
-        <f>I3&amp;J3&amp;K3&amp;L3&amp;M3&amp;N3&amp;O3&amp;P3&amp;Q3&amp;R3&amp;S3&amp;T3&amp;U3&amp;V3&amp;W3&amp;X3&amp;Y3&amp;Z3&amp;AA3</f>
-        <v>a = Post.new({caption: 'Boomer staring into the flames', location: ''', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_11.jpeg'), filename: '1_11.jpeg')a.save!</v>
+        <f t="shared" si="8"/>
+        <v>a = Post.new({caption: 'Boomer staring into the flames', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_11.jpeg'), filename: '1_11.jpeg')a.save!</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>80</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -3501,7 +3492,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="str">
-        <f>C4&amp;"_"&amp;D4&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>2_3.jpeg</v>
       </c>
       <c r="F4" t="s">
@@ -3511,7 +3502,7 @@
         <v>25</v>
       </c>
       <c r="H4">
-        <f>C4</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I4" t="s">
@@ -3521,7 +3512,7 @@
         <v>52</v>
       </c>
       <c r="K4" t="str">
-        <f>F4</f>
+        <f t="shared" si="3"/>
         <v>Zoom zoom Blue Angels</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -3531,7 +3522,7 @@
         <v>63</v>
       </c>
       <c r="N4" t="str">
-        <f>G4</f>
+        <f t="shared" si="4"/>
         <v>San Francisco, CA</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -3541,7 +3532,7 @@
         <v>64</v>
       </c>
       <c r="Q4">
-        <f>H4</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="R4" t="s">
@@ -3551,7 +3542,7 @@
         <v>55</v>
       </c>
       <c r="U4" t="str">
-        <f>E4</f>
+        <f t="shared" si="6"/>
         <v>2_3.jpeg</v>
       </c>
       <c r="V4" s="3" t="s">
@@ -3561,7 +3552,7 @@
         <v>56</v>
       </c>
       <c r="X4" t="str">
-        <f>E4</f>
+        <f t="shared" si="7"/>
         <v>2_3.jpeg</v>
       </c>
       <c r="Y4" s="3" t="s">
@@ -3571,14 +3562,14 @@
         <v>60</v>
       </c>
       <c r="AC4" t="str">
-        <f>I4&amp;J4&amp;K4&amp;L4&amp;M4&amp;N4&amp;O4&amp;P4&amp;Q4&amp;R4&amp;S4&amp;T4&amp;U4&amp;V4&amp;W4&amp;X4&amp;Y4&amp;Z4&amp;AA4</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Zoom zoom Blue Angels', location: 'San Francisco, CA', author_id: 2})a.photo.attach(io: File.open('app/assets/images/seed_images/2_3.jpeg'), filename: '2_3.jpeg')a.save!</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -3590,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <f>C5&amp;"_"&amp;D5&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>5_1.jpeg</v>
       </c>
       <c r="F5" t="s">
@@ -3600,7 +3591,7 @@
         <v>49</v>
       </c>
       <c r="H5">
-        <f>C5</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I5" t="s">
@@ -3610,7 +3601,7 @@
         <v>52</v>
       </c>
       <c r="K5" t="str">
-        <f>F5</f>
+        <f t="shared" si="3"/>
         <v>Arches</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -3620,7 +3611,7 @@
         <v>63</v>
       </c>
       <c r="N5" t="str">
-        <f>G5</f>
+        <f t="shared" si="4"/>
         <v>Arches National Park</v>
       </c>
       <c r="O5" s="3" t="s">
@@ -3630,7 +3621,7 @@
         <v>64</v>
       </c>
       <c r="Q5">
-        <f>H5</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="R5" t="s">
@@ -3640,7 +3631,7 @@
         <v>55</v>
       </c>
       <c r="U5" t="str">
-        <f>E5</f>
+        <f t="shared" si="6"/>
         <v>5_1.jpeg</v>
       </c>
       <c r="V5" s="3" t="s">
@@ -3650,7 +3641,7 @@
         <v>56</v>
       </c>
       <c r="X5" t="str">
-        <f>E5</f>
+        <f t="shared" si="7"/>
         <v>5_1.jpeg</v>
       </c>
       <c r="Y5" s="3" t="s">
@@ -3660,14 +3651,14 @@
         <v>60</v>
       </c>
       <c r="AC5" t="str">
-        <f>I5&amp;J5&amp;K5&amp;L5&amp;M5&amp;N5&amp;O5&amp;P5&amp;Q5&amp;R5&amp;S5&amp;T5&amp;U5&amp;V5&amp;W5&amp;X5&amp;Y5&amp;Z5&amp;AA5</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Arches', location: 'Arches National Park', author_id: 5})a.photo.attach(io: File.open('app/assets/images/seed_images/5_1.jpeg'), filename: '5_1.jpeg')a.save!</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>93</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -3679,7 +3670,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="str">
-        <f>C6&amp;"_"&amp;D6&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_13.jpeg</v>
       </c>
       <c r="F6" t="s">
@@ -3689,7 +3680,7 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <f>C6</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I6" t="s">
@@ -3699,7 +3690,7 @@
         <v>52</v>
       </c>
       <c r="K6" t="str">
-        <f>F6</f>
+        <f t="shared" si="3"/>
         <v>Snowy Firebird jump</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -3709,7 +3700,7 @@
         <v>63</v>
       </c>
       <c r="N6" t="str">
-        <f>G6</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O6" s="3" t="s">
@@ -3719,7 +3710,7 @@
         <v>64</v>
       </c>
       <c r="Q6">
-        <f>H6</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R6" t="s">
@@ -3729,7 +3720,7 @@
         <v>55</v>
       </c>
       <c r="U6" t="str">
-        <f>E6</f>
+        <f t="shared" si="6"/>
         <v>1_13.jpeg</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3739,7 +3730,7 @@
         <v>56</v>
       </c>
       <c r="X6" t="str">
-        <f>E6</f>
+        <f t="shared" si="7"/>
         <v>1_13.jpeg</v>
       </c>
       <c r="Y6" s="3" t="s">
@@ -3749,14 +3740,14 @@
         <v>60</v>
       </c>
       <c r="AC6" t="str">
-        <f>I6&amp;J6&amp;K6&amp;L6&amp;M6&amp;N6&amp;O6&amp;P6&amp;Q6&amp;R6&amp;S6&amp;T6&amp;U6&amp;V6&amp;W6&amp;X6&amp;Y6&amp;Z6&amp;AA6</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Snowy Firebird jump', location: 'Boston, MA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_13.jpeg'), filename: '1_13.jpeg')a.save!</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>57</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -3768,7 +3759,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="str">
-        <f>C7&amp;"_"&amp;D7&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_8.jpeg</v>
       </c>
       <c r="F7" t="s">
@@ -3778,7 +3769,7 @@
         <v>25</v>
       </c>
       <c r="H7">
-        <f>C7</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I7" t="s">
@@ -3788,7 +3779,7 @@
         <v>52</v>
       </c>
       <c r="K7" t="str">
-        <f>F7</f>
+        <f t="shared" si="3"/>
         <v>SF Golden Gate Bridge 🌉</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -3798,7 +3789,7 @@
         <v>63</v>
       </c>
       <c r="N7" t="str">
-        <f>G7</f>
+        <f t="shared" si="4"/>
         <v>San Francisco, CA</v>
       </c>
       <c r="O7" s="3" t="s">
@@ -3808,7 +3799,7 @@
         <v>64</v>
       </c>
       <c r="Q7">
-        <f>H7</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R7" t="s">
@@ -3818,7 +3809,7 @@
         <v>55</v>
       </c>
       <c r="U7" t="str">
-        <f>E7</f>
+        <f t="shared" si="6"/>
         <v>1_8.jpeg</v>
       </c>
       <c r="V7" s="3" t="s">
@@ -3828,7 +3819,7 @@
         <v>56</v>
       </c>
       <c r="X7" t="str">
-        <f>E7</f>
+        <f t="shared" si="7"/>
         <v>1_8.jpeg</v>
       </c>
       <c r="Y7" s="3" t="s">
@@ -3838,14 +3829,14 @@
         <v>60</v>
       </c>
       <c r="AC7" t="str">
-        <f>I7&amp;J7&amp;K7&amp;L7&amp;M7&amp;N7&amp;O7&amp;P7&amp;Q7&amp;R7&amp;S7&amp;T7&amp;U7&amp;V7&amp;W7&amp;X7&amp;Y7&amp;Z7&amp;AA7</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'SF Golden Gate Bridge 🌉', location: 'San Francisco, CA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_8.jpeg'), filename: '1_8.jpeg')a.save!</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>93</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -3857,7 +3848,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="str">
-        <f>C8&amp;"_"&amp;D8&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>4_3.jpeg</v>
       </c>
       <c r="F8" t="s">
@@ -3867,7 +3858,7 @@
         <v>44</v>
       </c>
       <c r="H8">
-        <f>C8</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I8" t="s">
@@ -3877,7 +3868,7 @@
         <v>52</v>
       </c>
       <c r="K8" t="str">
-        <f>F8</f>
+        <f t="shared" si="3"/>
         <v>Look at that!</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -3887,7 +3878,7 @@
         <v>63</v>
       </c>
       <c r="N8" t="str">
-        <f>G8</f>
+        <f t="shared" si="4"/>
         <v>Rocky National Park</v>
       </c>
       <c r="O8" s="3" t="s">
@@ -3897,7 +3888,7 @@
         <v>64</v>
       </c>
       <c r="Q8">
-        <f>H8</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="R8" t="s">
@@ -3907,7 +3898,7 @@
         <v>55</v>
       </c>
       <c r="U8" t="str">
-        <f>E8</f>
+        <f t="shared" si="6"/>
         <v>4_3.jpeg</v>
       </c>
       <c r="V8" s="3" t="s">
@@ -3917,7 +3908,7 @@
         <v>56</v>
       </c>
       <c r="X8" t="str">
-        <f>E8</f>
+        <f t="shared" si="7"/>
         <v>4_3.jpeg</v>
       </c>
       <c r="Y8" s="3" t="s">
@@ -3927,14 +3918,14 @@
         <v>60</v>
       </c>
       <c r="AC8" t="str">
-        <f>I8&amp;J8&amp;K8&amp;L8&amp;M8&amp;N8&amp;O8&amp;P8&amp;Q8&amp;R8&amp;S8&amp;T8&amp;U8&amp;V8&amp;W8&amp;X8&amp;Y8&amp;Z8&amp;AA8</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Look at that!', location: 'Rocky National Park', author_id: 4})a.photo.attach(io: File.open('app/assets/images/seed_images/4_3.jpeg'), filename: '4_3.jpeg')a.save!</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>13</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -3946,7 +3937,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="str">
-        <f>C9&amp;"_"&amp;D9&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_9.jpeg</v>
       </c>
       <c r="F9" t="s">
@@ -3956,7 +3947,7 @@
         <v>15</v>
       </c>
       <c r="H9">
-        <f>C9</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I9" t="s">
@@ -3966,7 +3957,7 @@
         <v>52</v>
       </c>
       <c r="K9" t="str">
-        <f>F9</f>
+        <f t="shared" si="3"/>
         <v>Boston Night from above</v>
       </c>
       <c r="L9" s="3" t="s">
@@ -3976,7 +3967,7 @@
         <v>63</v>
       </c>
       <c r="N9" t="str">
-        <f>G9</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O9" s="3" t="s">
@@ -3986,7 +3977,7 @@
         <v>64</v>
       </c>
       <c r="Q9">
-        <f>H9</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R9" t="s">
@@ -3996,7 +3987,7 @@
         <v>55</v>
       </c>
       <c r="U9" t="str">
-        <f>E9</f>
+        <f t="shared" si="6"/>
         <v>1_9.jpeg</v>
       </c>
       <c r="V9" s="3" t="s">
@@ -4006,7 +3997,7 @@
         <v>56</v>
       </c>
       <c r="X9" t="str">
-        <f>E9</f>
+        <f t="shared" si="7"/>
         <v>1_9.jpeg</v>
       </c>
       <c r="Y9" s="3" t="s">
@@ -4016,14 +4007,14 @@
         <v>60</v>
       </c>
       <c r="AC9" t="str">
-        <f>I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9&amp;O9&amp;P9&amp;Q9&amp;R9&amp;S9&amp;T9&amp;U9&amp;V9&amp;W9&amp;X9&amp;Y9&amp;Z9&amp;AA9</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Boston Night from above', location: 'Boston, MA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_9.jpeg'), filename: '1_9.jpeg')a.save!</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>79</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -4035,7 +4026,7 @@
         <v>2</v>
       </c>
       <c r="E10" t="str">
-        <f>C10&amp;"_"&amp;D10&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>4_2.jpeg</v>
       </c>
       <c r="F10" t="s">
@@ -4045,7 +4036,7 @@
         <v>44</v>
       </c>
       <c r="H10">
-        <f>C10</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I10" t="s">
@@ -4055,7 +4046,7 @@
         <v>52</v>
       </c>
       <c r="K10" t="str">
-        <f>F10</f>
+        <f t="shared" si="3"/>
         <v>Waaaaaaa</v>
       </c>
       <c r="L10" s="3" t="s">
@@ -4065,7 +4056,7 @@
         <v>63</v>
       </c>
       <c r="N10" t="str">
-        <f>G10</f>
+        <f t="shared" si="4"/>
         <v>Rocky National Park</v>
       </c>
       <c r="O10" s="3" t="s">
@@ -4075,7 +4066,7 @@
         <v>64</v>
       </c>
       <c r="Q10">
-        <f>H10</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="R10" t="s">
@@ -4085,7 +4076,7 @@
         <v>55</v>
       </c>
       <c r="U10" t="str">
-        <f>E10</f>
+        <f t="shared" si="6"/>
         <v>4_2.jpeg</v>
       </c>
       <c r="V10" s="3" t="s">
@@ -4095,7 +4086,7 @@
         <v>56</v>
       </c>
       <c r="X10" t="str">
-        <f>E10</f>
+        <f t="shared" si="7"/>
         <v>4_2.jpeg</v>
       </c>
       <c r="Y10" s="3" t="s">
@@ -4105,14 +4096,14 @@
         <v>60</v>
       </c>
       <c r="AC10" t="str">
-        <f>I10&amp;J10&amp;K10&amp;L10&amp;M10&amp;N10&amp;O10&amp;P10&amp;Q10&amp;R10&amp;S10&amp;T10&amp;U10&amp;V10&amp;W10&amp;X10&amp;Y10&amp;Z10&amp;AA10</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Waaaaaaa', location: 'Rocky National Park', author_id: 4})a.photo.attach(io: File.open('app/assets/images/seed_images/4_2.jpeg'), filename: '4_2.jpeg')a.save!</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>87</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -4124,7 +4115,7 @@
         <v>5</v>
       </c>
       <c r="E11" t="str">
-        <f>C11&amp;"_"&amp;D11&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_5.jpeg</v>
       </c>
       <c r="F11" t="s">
@@ -4134,7 +4125,7 @@
         <v>15</v>
       </c>
       <c r="H11">
-        <f>C11</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I11" t="s">
@@ -4144,7 +4135,7 @@
         <v>52</v>
       </c>
       <c r="K11" t="str">
-        <f>F11</f>
+        <f t="shared" si="3"/>
         <v>B&lt;3ston</v>
       </c>
       <c r="L11" s="3" t="s">
@@ -4154,7 +4145,7 @@
         <v>63</v>
       </c>
       <c r="N11" t="str">
-        <f>G11</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O11" s="3" t="s">
@@ -4164,7 +4155,7 @@
         <v>64</v>
       </c>
       <c r="Q11">
-        <f>H11</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R11" t="s">
@@ -4174,7 +4165,7 @@
         <v>55</v>
       </c>
       <c r="U11" t="str">
-        <f>E11</f>
+        <f t="shared" si="6"/>
         <v>1_5.jpeg</v>
       </c>
       <c r="V11" s="3" t="s">
@@ -4184,7 +4175,7 @@
         <v>56</v>
       </c>
       <c r="X11" t="str">
-        <f>E11</f>
+        <f t="shared" si="7"/>
         <v>1_5.jpeg</v>
       </c>
       <c r="Y11" s="3" t="s">
@@ -4194,14 +4185,14 @@
         <v>60</v>
       </c>
       <c r="AC11" t="str">
-        <f>I11&amp;J11&amp;K11&amp;L11&amp;M11&amp;N11&amp;O11&amp;P11&amp;Q11&amp;R11&amp;S11&amp;T11&amp;U11&amp;V11&amp;W11&amp;X11&amp;Y11&amp;Z11&amp;AA11</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'B&lt;3ston', location: 'Boston, MA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_5.jpeg'), filename: '1_5.jpeg')a.save!</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>28</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -4213,7 +4204,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="str">
-        <f>C12&amp;"_"&amp;D12&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_4.jpeg</v>
       </c>
       <c r="F12" t="s">
@@ -4223,7 +4214,7 @@
         <v>15</v>
       </c>
       <c r="H12">
-        <f>C12</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I12" t="s">
@@ -4233,7 +4224,7 @@
         <v>52</v>
       </c>
       <c r="K12" t="str">
-        <f>F12</f>
+        <f t="shared" si="3"/>
         <v>Peek-a-Boston</v>
       </c>
       <c r="L12" s="3" t="s">
@@ -4243,7 +4234,7 @@
         <v>63</v>
       </c>
       <c r="N12" t="str">
-        <f>G12</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O12" s="3" t="s">
@@ -4253,7 +4244,7 @@
         <v>64</v>
       </c>
       <c r="Q12">
-        <f>H12</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R12" t="s">
@@ -4263,7 +4254,7 @@
         <v>55</v>
       </c>
       <c r="U12" t="str">
-        <f>E12</f>
+        <f t="shared" si="6"/>
         <v>1_4.jpeg</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -4273,7 +4264,7 @@
         <v>56</v>
       </c>
       <c r="X12" t="str">
-        <f>E12</f>
+        <f t="shared" si="7"/>
         <v>1_4.jpeg</v>
       </c>
       <c r="Y12" s="3" t="s">
@@ -4283,14 +4274,14 @@
         <v>60</v>
       </c>
       <c r="AC12" t="str">
-        <f>I12&amp;J12&amp;K12&amp;L12&amp;M12&amp;N12&amp;O12&amp;P12&amp;Q12&amp;R12&amp;S12&amp;T12&amp;U12&amp;V12&amp;W12&amp;X12&amp;Y12&amp;Z12&amp;AA12</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Peek-a-Boston', location: 'Boston, MA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_4.jpeg'), filename: '1_4.jpeg')a.save!</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>89</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -4302,7 +4293,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="str">
-        <f>C13&amp;"_"&amp;D13&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_14.jpeg</v>
       </c>
       <c r="F13" t="s">
@@ -4312,7 +4303,7 @@
         <v>15</v>
       </c>
       <c r="H13">
-        <f>C13</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I13" t="s">
@@ -4322,7 +4313,7 @@
         <v>52</v>
       </c>
       <c r="K13" t="str">
-        <f>F13</f>
+        <f t="shared" si="3"/>
         <v>Make way for the Ducklings</v>
       </c>
       <c r="L13" s="3" t="s">
@@ -4332,7 +4323,7 @@
         <v>63</v>
       </c>
       <c r="N13" t="str">
-        <f>G13</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O13" s="3" t="s">
@@ -4342,7 +4333,7 @@
         <v>64</v>
       </c>
       <c r="Q13">
-        <f>H13</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R13" t="s">
@@ -4352,7 +4343,7 @@
         <v>55</v>
       </c>
       <c r="U13" t="str">
-        <f>E13</f>
+        <f t="shared" si="6"/>
         <v>1_14.jpeg</v>
       </c>
       <c r="V13" s="3" t="s">
@@ -4362,7 +4353,7 @@
         <v>56</v>
       </c>
       <c r="X13" t="str">
-        <f>E13</f>
+        <f t="shared" si="7"/>
         <v>1_14.jpeg</v>
       </c>
       <c r="Y13" s="3" t="s">
@@ -4372,14 +4363,14 @@
         <v>60</v>
       </c>
       <c r="AC13" t="str">
-        <f>I13&amp;J13&amp;K13&amp;L13&amp;M13&amp;N13&amp;O13&amp;P13&amp;Q13&amp;R13&amp;S13&amp;T13&amp;U13&amp;V13&amp;W13&amp;X13&amp;Y13&amp;Z13&amp;AA13</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Make way for the Ducklings', location: 'Boston, MA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_14.jpeg'), filename: '1_14.jpeg')a.save!</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>94</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -4391,7 +4382,7 @@
         <v>3</v>
       </c>
       <c r="E14" t="str">
-        <f>C14&amp;"_"&amp;D14&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>3_3.jpeg</v>
       </c>
       <c r="F14" t="s">
@@ -4401,7 +4392,7 @@
         <v>33</v>
       </c>
       <c r="H14">
-        <f>C14</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I14" t="s">
@@ -4411,7 +4402,7 @@
         <v>52</v>
       </c>
       <c r="K14" t="str">
-        <f>F14</f>
+        <f t="shared" si="3"/>
         <v>Vernazza!</v>
       </c>
       <c r="L14" s="3" t="s">
@@ -4421,7 +4412,7 @@
         <v>63</v>
       </c>
       <c r="N14" t="str">
-        <f>G14</f>
+        <f t="shared" si="4"/>
         <v>Cinque Terre, Italy</v>
       </c>
       <c r="O14" s="3" t="s">
@@ -4431,7 +4422,7 @@
         <v>64</v>
       </c>
       <c r="Q14">
-        <f>H14</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="R14" t="s">
@@ -4441,7 +4432,7 @@
         <v>55</v>
       </c>
       <c r="U14" t="str">
-        <f>E14</f>
+        <f t="shared" si="6"/>
         <v>3_3.jpeg</v>
       </c>
       <c r="V14" s="3" t="s">
@@ -4451,7 +4442,7 @@
         <v>56</v>
       </c>
       <c r="X14" t="str">
-        <f>E14</f>
+        <f t="shared" si="7"/>
         <v>3_3.jpeg</v>
       </c>
       <c r="Y14" s="3" t="s">
@@ -4461,14 +4452,14 @@
         <v>60</v>
       </c>
       <c r="AC14" t="str">
-        <f>I14&amp;J14&amp;K14&amp;L14&amp;M14&amp;N14&amp;O14&amp;P14&amp;Q14&amp;R14&amp;S14&amp;T14&amp;U14&amp;V14&amp;W14&amp;X14&amp;Y14&amp;Z14&amp;AA14</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Vernazza!', location: 'Cinque Terre, Italy', author_id: 3})a.photo.attach(io: File.open('app/assets/images/seed_images/3_3.jpeg'), filename: '3_3.jpeg')a.save!</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -4480,7 +4471,7 @@
         <v>2</v>
       </c>
       <c r="E15" t="str">
-        <f>C15&amp;"_"&amp;D15&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>2_2.jpeg</v>
       </c>
       <c r="F15" t="s">
@@ -4490,7 +4481,7 @@
         <v>37</v>
       </c>
       <c r="H15">
-        <f>C15</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I15" t="s">
@@ -4500,7 +4491,7 @@
         <v>52</v>
       </c>
       <c r="K15" t="str">
-        <f>F15</f>
+        <f t="shared" si="3"/>
         <v>The U Bend.</v>
       </c>
       <c r="L15" s="3" t="s">
@@ -4510,7 +4501,7 @@
         <v>63</v>
       </c>
       <c r="N15" t="str">
-        <f>G15</f>
+        <f t="shared" si="4"/>
         <v>Horseshoe Bend</v>
       </c>
       <c r="O15" s="3" t="s">
@@ -4520,7 +4511,7 @@
         <v>64</v>
       </c>
       <c r="Q15">
-        <f>H15</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="R15" t="s">
@@ -4530,7 +4521,7 @@
         <v>55</v>
       </c>
       <c r="U15" t="str">
-        <f>E15</f>
+        <f t="shared" si="6"/>
         <v>2_2.jpeg</v>
       </c>
       <c r="V15" s="3" t="s">
@@ -4540,7 +4531,7 @@
         <v>56</v>
       </c>
       <c r="X15" t="str">
-        <f>E15</f>
+        <f t="shared" si="7"/>
         <v>2_2.jpeg</v>
       </c>
       <c r="Y15" s="3" t="s">
@@ -4550,14 +4541,14 @@
         <v>60</v>
       </c>
       <c r="AC15" t="str">
-        <f>I15&amp;J15&amp;K15&amp;L15&amp;M15&amp;N15&amp;O15&amp;P15&amp;Q15&amp;R15&amp;S15&amp;T15&amp;U15&amp;V15&amp;W15&amp;X15&amp;Y15&amp;Z15&amp;AA15</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'The U Bend.', location: 'Horseshoe Bend', author_id: 2})a.photo.attach(io: File.open('app/assets/images/seed_images/2_2.jpeg'), filename: '2_2.jpeg')a.save!</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>69</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -4569,7 +4560,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="str">
-        <f>C16&amp;"_"&amp;D16&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_1.jpeg</v>
       </c>
       <c r="F16" t="s">
@@ -4579,7 +4570,7 @@
         <v>15</v>
       </c>
       <c r="H16">
-        <f>C16</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I16" t="s">
@@ -4589,7 +4580,7 @@
         <v>52</v>
       </c>
       <c r="K16" t="str">
-        <f>F16</f>
+        <f t="shared" si="3"/>
         <v>Boston Sails by the Charles</v>
       </c>
       <c r="L16" s="3" t="s">
@@ -4599,7 +4590,7 @@
         <v>63</v>
       </c>
       <c r="N16" t="str">
-        <f>G16</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O16" s="3" t="s">
@@ -4609,7 +4600,7 @@
         <v>64</v>
       </c>
       <c r="Q16">
-        <f>H16</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R16" t="s">
@@ -4619,7 +4610,7 @@
         <v>55</v>
       </c>
       <c r="U16" t="str">
-        <f>E16</f>
+        <f t="shared" si="6"/>
         <v>1_1.jpeg</v>
       </c>
       <c r="V16" s="3" t="s">
@@ -4629,7 +4620,7 @@
         <v>56</v>
       </c>
       <c r="X16" t="str">
-        <f>E16</f>
+        <f t="shared" si="7"/>
         <v>1_1.jpeg</v>
       </c>
       <c r="Y16" s="3" t="s">
@@ -4639,14 +4630,14 @@
         <v>60</v>
       </c>
       <c r="AC16" t="str">
-        <f>I16&amp;J16&amp;K16&amp;L16&amp;M16&amp;N16&amp;O16&amp;P16&amp;Q16&amp;R16&amp;S16&amp;T16&amp;U16&amp;V16&amp;W16&amp;X16&amp;Y16&amp;Z16&amp;AA16</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Boston Sails by the Charles', location: 'Boston, MA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_1.jpeg'), filename: '1_1.jpeg')a.save!</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>70</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -4658,7 +4649,7 @@
         <v>4</v>
       </c>
       <c r="E17" t="str">
-        <f>C17&amp;"_"&amp;D17&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>4_4.jpeg</v>
       </c>
       <c r="F17" t="s">
@@ -4668,7 +4659,7 @@
         <v>25</v>
       </c>
       <c r="H17">
-        <f>C17</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I17" t="s">
@@ -4678,7 +4669,7 @@
         <v>52</v>
       </c>
       <c r="K17" t="str">
-        <f>F17</f>
+        <f t="shared" si="3"/>
         <v>Swinging away</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -4688,7 +4679,7 @@
         <v>63</v>
       </c>
       <c r="N17" t="str">
-        <f>G17</f>
+        <f t="shared" si="4"/>
         <v>San Francisco, CA</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -4698,7 +4689,7 @@
         <v>64</v>
       </c>
       <c r="Q17">
-        <f>H17</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="R17" t="s">
@@ -4708,7 +4699,7 @@
         <v>55</v>
       </c>
       <c r="U17" t="str">
-        <f>E17</f>
+        <f t="shared" si="6"/>
         <v>4_4.jpeg</v>
       </c>
       <c r="V17" s="3" t="s">
@@ -4718,7 +4709,7 @@
         <v>56</v>
       </c>
       <c r="X17" t="str">
-        <f>E17</f>
+        <f t="shared" si="7"/>
         <v>4_4.jpeg</v>
       </c>
       <c r="Y17" s="3" t="s">
@@ -4728,14 +4719,14 @@
         <v>60</v>
       </c>
       <c r="AC17" t="str">
-        <f>I17&amp;J17&amp;K17&amp;L17&amp;M17&amp;N17&amp;O17&amp;P17&amp;Q17&amp;R17&amp;S17&amp;T17&amp;U17&amp;V17&amp;W17&amp;X17&amp;Y17&amp;Z17&amp;AA17</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Swinging away', location: 'San Francisco, CA', author_id: 4})a.photo.attach(io: File.open('app/assets/images/seed_images/4_4.jpeg'), filename: '4_4.jpeg')a.save!</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>69</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -4747,7 +4738,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="str">
-        <f>C18&amp;"_"&amp;D18&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>4_1.jpeg</v>
       </c>
       <c r="F18" t="s">
@@ -4757,7 +4748,7 @@
         <v>17</v>
       </c>
       <c r="H18">
-        <f>C18</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I18" t="s">
@@ -4767,7 +4758,7 @@
         <v>52</v>
       </c>
       <c r="K18" t="str">
-        <f>F18</f>
+        <f t="shared" si="3"/>
         <v>Weeeeee</v>
       </c>
       <c r="L18" s="3" t="s">
@@ -4777,7 +4768,7 @@
         <v>63</v>
       </c>
       <c r="N18" t="str">
-        <f>G18</f>
+        <f t="shared" si="4"/>
         <v>Amsterdam. Netherlands</v>
       </c>
       <c r="O18" s="3" t="s">
@@ -4787,7 +4778,7 @@
         <v>64</v>
       </c>
       <c r="Q18">
-        <f>H18</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="R18" t="s">
@@ -4797,7 +4788,7 @@
         <v>55</v>
       </c>
       <c r="U18" t="str">
-        <f>E18</f>
+        <f t="shared" si="6"/>
         <v>4_1.jpeg</v>
       </c>
       <c r="V18" s="3" t="s">
@@ -4807,7 +4798,7 @@
         <v>56</v>
       </c>
       <c r="X18" t="str">
-        <f>E18</f>
+        <f t="shared" si="7"/>
         <v>4_1.jpeg</v>
       </c>
       <c r="Y18" s="3" t="s">
@@ -4817,14 +4808,14 @@
         <v>60</v>
       </c>
       <c r="AC18" t="str">
-        <f>I18&amp;J18&amp;K18&amp;L18&amp;M18&amp;N18&amp;O18&amp;P18&amp;Q18&amp;R18&amp;S18&amp;T18&amp;U18&amp;V18&amp;W18&amp;X18&amp;Y18&amp;Z18&amp;AA18</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Weeeeee', location: 'Amsterdam. Netherlands', author_id: 4})a.photo.attach(io: File.open('app/assets/images/seed_images/4_1.jpeg'), filename: '4_1.jpeg')a.save!</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>86</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -4836,7 +4827,7 @@
         <v>5</v>
       </c>
       <c r="E19" t="str">
-        <f>C19&amp;"_"&amp;D19&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>4_5.jpeg</v>
       </c>
       <c r="F19" t="s">
@@ -4846,7 +4837,7 @@
         <v>33</v>
       </c>
       <c r="H19">
-        <f>C19</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I19" t="s">
@@ -4856,7 +4847,7 @@
         <v>52</v>
       </c>
       <c r="K19" t="str">
-        <f>F19</f>
+        <f t="shared" si="3"/>
         <v>Hidden path</v>
       </c>
       <c r="L19" s="3" t="s">
@@ -4866,7 +4857,7 @@
         <v>63</v>
       </c>
       <c r="N19" t="str">
-        <f>G19</f>
+        <f t="shared" si="4"/>
         <v>Cinque Terre, Italy</v>
       </c>
       <c r="O19" s="3" t="s">
@@ -4876,7 +4867,7 @@
         <v>64</v>
       </c>
       <c r="Q19">
-        <f>H19</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="R19" t="s">
@@ -4886,7 +4877,7 @@
         <v>55</v>
       </c>
       <c r="U19" t="str">
-        <f>E19</f>
+        <f t="shared" si="6"/>
         <v>4_5.jpeg</v>
       </c>
       <c r="V19" s="3" t="s">
@@ -4896,7 +4887,7 @@
         <v>56</v>
       </c>
       <c r="X19" t="str">
-        <f>E19</f>
+        <f t="shared" si="7"/>
         <v>4_5.jpeg</v>
       </c>
       <c r="Y19" s="3" t="s">
@@ -4906,14 +4897,14 @@
         <v>60</v>
       </c>
       <c r="AC19" t="str">
-        <f>I19&amp;J19&amp;K19&amp;L19&amp;M19&amp;N19&amp;O19&amp;P19&amp;Q19&amp;R19&amp;S19&amp;T19&amp;U19&amp;V19&amp;W19&amp;X19&amp;Y19&amp;Z19&amp;AA19</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Hidden path', location: 'Cinque Terre, Italy', author_id: 4})a.photo.attach(io: File.open('app/assets/images/seed_images/4_5.jpeg'), filename: '4_5.jpeg')a.save!</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>36</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -4925,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="str">
-        <f>C20&amp;"_"&amp;D20&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>3_1.jpeg</v>
       </c>
       <c r="F20" t="s">
@@ -4935,7 +4926,7 @@
         <v>15</v>
       </c>
       <c r="H20">
-        <f>C20</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I20" t="s">
@@ -4945,7 +4936,7 @@
         <v>52</v>
       </c>
       <c r="K20" t="str">
-        <f>F20</f>
+        <f t="shared" si="3"/>
         <v>Boston from BU</v>
       </c>
       <c r="L20" s="3" t="s">
@@ -4955,7 +4946,7 @@
         <v>63</v>
       </c>
       <c r="N20" t="str">
-        <f>G20</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O20" s="3" t="s">
@@ -4965,7 +4956,7 @@
         <v>64</v>
       </c>
       <c r="Q20">
-        <f>H20</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="R20" t="s">
@@ -4975,7 +4966,7 @@
         <v>55</v>
       </c>
       <c r="U20" t="str">
-        <f>E20</f>
+        <f t="shared" si="6"/>
         <v>3_1.jpeg</v>
       </c>
       <c r="V20" s="3" t="s">
@@ -4985,7 +4976,7 @@
         <v>56</v>
       </c>
       <c r="X20" t="str">
-        <f>E20</f>
+        <f t="shared" si="7"/>
         <v>3_1.jpeg</v>
       </c>
       <c r="Y20" s="3" t="s">
@@ -4995,14 +4986,14 @@
         <v>60</v>
       </c>
       <c r="AC20" t="str">
-        <f>I20&amp;J20&amp;K20&amp;L20&amp;M20&amp;N20&amp;O20&amp;P20&amp;Q20&amp;R20&amp;S20&amp;T20&amp;U20&amp;V20&amp;W20&amp;X20&amp;Y20&amp;Z20&amp;AA20</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Boston from BU', location: 'Boston, MA', author_id: 3})a.photo.attach(io: File.open('app/assets/images/seed_images/3_1.jpeg'), filename: '3_1.jpeg')a.save!</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -5014,7 +5005,7 @@
         <v>15</v>
       </c>
       <c r="E21" t="str">
-        <f>C21&amp;"_"&amp;D21&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_15.jpeg</v>
       </c>
       <c r="F21" t="s">
@@ -5024,7 +5015,7 @@
         <v>33</v>
       </c>
       <c r="H21">
-        <f>C21</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I21" t="s">
@@ -5034,7 +5025,7 @@
         <v>52</v>
       </c>
       <c r="K21" t="str">
-        <f>F21</f>
+        <f t="shared" si="3"/>
         <v>Vivid coastal village</v>
       </c>
       <c r="L21" s="3" t="s">
@@ -5044,7 +5035,7 @@
         <v>63</v>
       </c>
       <c r="N21" t="str">
-        <f>G21</f>
+        <f t="shared" si="4"/>
         <v>Cinque Terre, Italy</v>
       </c>
       <c r="O21" s="3" t="s">
@@ -5054,7 +5045,7 @@
         <v>64</v>
       </c>
       <c r="Q21">
-        <f>H21</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R21" t="s">
@@ -5064,7 +5055,7 @@
         <v>55</v>
       </c>
       <c r="U21" t="str">
-        <f>E21</f>
+        <f t="shared" si="6"/>
         <v>1_15.jpeg</v>
       </c>
       <c r="V21" s="3" t="s">
@@ -5074,7 +5065,7 @@
         <v>56</v>
       </c>
       <c r="X21" t="str">
-        <f>E21</f>
+        <f t="shared" si="7"/>
         <v>1_15.jpeg</v>
       </c>
       <c r="Y21" s="3" t="s">
@@ -5084,14 +5075,14 @@
         <v>60</v>
       </c>
       <c r="AC21" t="str">
-        <f>I21&amp;J21&amp;K21&amp;L21&amp;M21&amp;N21&amp;O21&amp;P21&amp;Q21&amp;R21&amp;S21&amp;T21&amp;U21&amp;V21&amp;W21&amp;X21&amp;Y21&amp;Z21&amp;AA21</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Vivid coastal village', location: 'Cinque Terre, Italy', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_15.jpeg'), filename: '1_15.jpeg')a.save!</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>40</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -5103,7 +5094,7 @@
         <v>3</v>
       </c>
       <c r="E22" t="str">
-        <f>C22&amp;"_"&amp;D22&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_3.jpeg</v>
       </c>
       <c r="F22" t="s">
@@ -5113,7 +5104,7 @@
         <v>17</v>
       </c>
       <c r="H22">
-        <f>C22</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I22" t="s">
@@ -5123,7 +5114,7 @@
         <v>52</v>
       </c>
       <c r="K22" t="str">
-        <f>F22</f>
+        <f t="shared" si="3"/>
         <v>iAmsterdam</v>
       </c>
       <c r="L22" s="3" t="s">
@@ -5133,7 +5124,7 @@
         <v>63</v>
       </c>
       <c r="N22" t="str">
-        <f>G22</f>
+        <f t="shared" si="4"/>
         <v>Amsterdam. Netherlands</v>
       </c>
       <c r="O22" s="3" t="s">
@@ -5143,7 +5134,7 @@
         <v>64</v>
       </c>
       <c r="Q22">
-        <f>H22</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R22" t="s">
@@ -5153,7 +5144,7 @@
         <v>55</v>
       </c>
       <c r="U22" t="str">
-        <f>E22</f>
+        <f t="shared" si="6"/>
         <v>1_3.jpeg</v>
       </c>
       <c r="V22" s="3" t="s">
@@ -5163,7 +5154,7 @@
         <v>56</v>
       </c>
       <c r="X22" t="str">
-        <f>E22</f>
+        <f t="shared" si="7"/>
         <v>1_3.jpeg</v>
       </c>
       <c r="Y22" s="3" t="s">
@@ -5173,14 +5164,14 @@
         <v>60</v>
       </c>
       <c r="AC22" t="str">
-        <f>I22&amp;J22&amp;K22&amp;L22&amp;M22&amp;N22&amp;O22&amp;P22&amp;Q22&amp;R22&amp;S22&amp;T22&amp;U22&amp;V22&amp;W22&amp;X22&amp;Y22&amp;Z22&amp;AA22</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'iAmsterdam', location: 'Amsterdam. Netherlands', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_3.jpeg'), filename: '1_3.jpeg')a.save!</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>83</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -5192,7 +5183,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="str">
-        <f>C23&amp;"_"&amp;D23&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_10.jpeg</v>
       </c>
       <c r="F23" t="s">
@@ -5202,7 +5193,7 @@
         <v>28</v>
       </c>
       <c r="H23">
-        <f>C23</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I23" t="s">
@@ -5212,7 +5203,7 @@
         <v>52</v>
       </c>
       <c r="K23" t="str">
-        <f>F23</f>
+        <f t="shared" si="3"/>
         <v>Zion Overlook</v>
       </c>
       <c r="L23" s="3" t="s">
@@ -5222,7 +5213,7 @@
         <v>63</v>
       </c>
       <c r="N23" t="str">
-        <f>G23</f>
+        <f t="shared" si="4"/>
         <v>Zion National Park</v>
       </c>
       <c r="O23" s="3" t="s">
@@ -5232,7 +5223,7 @@
         <v>64</v>
       </c>
       <c r="Q23">
-        <f>H23</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R23" t="s">
@@ -5242,7 +5233,7 @@
         <v>55</v>
       </c>
       <c r="U23" t="str">
-        <f>E23</f>
+        <f t="shared" si="6"/>
         <v>1_10.jpeg</v>
       </c>
       <c r="V23" s="3" t="s">
@@ -5252,7 +5243,7 @@
         <v>56</v>
       </c>
       <c r="X23" t="str">
-        <f>E23</f>
+        <f t="shared" si="7"/>
         <v>1_10.jpeg</v>
       </c>
       <c r="Y23" s="3" t="s">
@@ -5262,13 +5253,13 @@
         <v>60</v>
       </c>
       <c r="AC23" t="str">
-        <f>I23&amp;J23&amp;K23&amp;L23&amp;M23&amp;N23&amp;O23&amp;P23&amp;Q23&amp;R23&amp;S23&amp;T23&amp;U23&amp;V23&amp;W23&amp;X23&amp;Y23&amp;Z23&amp;AA23</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Zion Overlook', location: 'Zion National Park', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_10.jpeg'), filename: '1_10.jpeg')a.save!</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f ca="1">RANDBETWEEN(1,100)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
       <c r="B24">
@@ -5281,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="str">
-        <f>C24&amp;"_"&amp;D24&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_2.jpeg</v>
       </c>
       <c r="F24" t="s">
@@ -5291,7 +5282,7 @@
         <v>17</v>
       </c>
       <c r="H24">
-        <f>C24</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I24" t="s">
@@ -5301,7 +5292,7 @@
         <v>52</v>
       </c>
       <c r="K24" t="str">
-        <f>F24</f>
+        <f t="shared" si="3"/>
         <v>Bottle from Amsterdam</v>
       </c>
       <c r="L24" s="3" t="s">
@@ -5311,7 +5302,7 @@
         <v>63</v>
       </c>
       <c r="N24" t="str">
-        <f>G24</f>
+        <f t="shared" si="4"/>
         <v>Amsterdam. Netherlands</v>
       </c>
       <c r="O24" s="3" t="s">
@@ -5321,7 +5312,7 @@
         <v>64</v>
       </c>
       <c r="Q24">
-        <f>H24</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R24" t="s">
@@ -5331,7 +5322,7 @@
         <v>55</v>
       </c>
       <c r="U24" t="str">
-        <f>E24</f>
+        <f t="shared" si="6"/>
         <v>1_2.jpeg</v>
       </c>
       <c r="V24" s="3" t="s">
@@ -5341,7 +5332,7 @@
         <v>56</v>
       </c>
       <c r="X24" t="str">
-        <f>E24</f>
+        <f t="shared" si="7"/>
         <v>1_2.jpeg</v>
       </c>
       <c r="Y24" s="3" t="s">
@@ -5351,14 +5342,14 @@
         <v>60</v>
       </c>
       <c r="AC24" t="str">
-        <f>I24&amp;J24&amp;K24&amp;L24&amp;M24&amp;N24&amp;O24&amp;P24&amp;Q24&amp;R24&amp;S24&amp;T24&amp;U24&amp;V24&amp;W24&amp;X24&amp;Y24&amp;Z24&amp;AA24</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Bottle from Amsterdam', location: 'Amsterdam. Netherlands', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_2.jpeg'), filename: '1_2.jpeg')a.save!</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -5370,7 +5361,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f>C25&amp;"_"&amp;D25&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_7.jpeg</v>
       </c>
       <c r="F25" t="s">
@@ -5380,7 +5371,7 @@
         <v>15</v>
       </c>
       <c r="H25">
-        <f>C25</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I25" t="s">
@@ -5390,7 +5381,7 @@
         <v>52</v>
       </c>
       <c r="K25" t="str">
-        <f>F25</f>
+        <f t="shared" si="3"/>
         <v>Boston from Longsfellow</v>
       </c>
       <c r="L25" s="3" t="s">
@@ -5400,7 +5391,7 @@
         <v>63</v>
       </c>
       <c r="N25" t="str">
-        <f>G25</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -5410,7 +5401,7 @@
         <v>64</v>
       </c>
       <c r="Q25">
-        <f>H25</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R25" t="s">
@@ -5420,7 +5411,7 @@
         <v>55</v>
       </c>
       <c r="U25" t="str">
-        <f>E25</f>
+        <f t="shared" si="6"/>
         <v>1_7.jpeg</v>
       </c>
       <c r="V25" s="3" t="s">
@@ -5430,7 +5421,7 @@
         <v>56</v>
       </c>
       <c r="X25" t="str">
-        <f>E25</f>
+        <f t="shared" si="7"/>
         <v>1_7.jpeg</v>
       </c>
       <c r="Y25" s="3" t="s">
@@ -5440,14 +5431,14 @@
         <v>60</v>
       </c>
       <c r="AC25" t="str">
-        <f>I25&amp;J25&amp;K25&amp;L25&amp;M25&amp;N25&amp;O25&amp;P25&amp;Q25&amp;R25&amp;S25&amp;T25&amp;U25&amp;V25&amp;W25&amp;X25&amp;Y25&amp;Z25&amp;AA25</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Boston from Longsfellow', location: 'Boston, MA', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_7.jpeg'), filename: '1_7.jpeg')a.save!</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -5459,7 +5450,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="str">
-        <f>C26&amp;"_"&amp;D26&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>2_1.jpeg</v>
       </c>
       <c r="F26" t="s">
@@ -5469,7 +5460,7 @@
         <v>68</v>
       </c>
       <c r="H26">
-        <f>C26</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I26" t="s">
@@ -5479,27 +5470,18 @@
         <v>52</v>
       </c>
       <c r="K26" t="str">
-        <f>F26</f>
+        <f t="shared" si="3"/>
         <v>Lets pool</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M26" t="s">
-        <v>63</v>
-      </c>
-      <c r="N26" t="str">
-        <f>G26</f>
-        <v>'</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="O26" s="3"/>
       <c r="P26" t="s">
         <v>64</v>
       </c>
       <c r="Q26">
-        <f>H26</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="R26" t="s">
@@ -5509,7 +5491,7 @@
         <v>55</v>
       </c>
       <c r="U26" t="str">
-        <f>E26</f>
+        <f t="shared" si="6"/>
         <v>2_1.jpeg</v>
       </c>
       <c r="V26" s="3" t="s">
@@ -5519,7 +5501,7 @@
         <v>56</v>
       </c>
       <c r="X26" t="str">
-        <f>E26</f>
+        <f t="shared" si="7"/>
         <v>2_1.jpeg</v>
       </c>
       <c r="Y26" s="3" t="s">
@@ -5529,14 +5511,14 @@
         <v>60</v>
       </c>
       <c r="AC26" t="str">
-        <f>I26&amp;J26&amp;K26&amp;L26&amp;M26&amp;N26&amp;O26&amp;P26&amp;Q26&amp;R26&amp;S26&amp;T26&amp;U26&amp;V26&amp;W26&amp;X26&amp;Y26&amp;Z26&amp;AA26</f>
-        <v>a = Post.new({caption: 'Lets pool', location: ''', author_id: 2})a.photo.attach(io: File.open('app/assets/images/seed_images/2_1.jpeg'), filename: '2_1.jpeg')a.save!</v>
+        <f t="shared" si="8"/>
+        <v>a = Post.new({caption: 'Lets pool', author_id: 2})a.photo.attach(io: File.open('app/assets/images/seed_images/2_1.jpeg'), filename: '2_1.jpeg')a.save!</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>75</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -5548,7 +5530,7 @@
         <v>12</v>
       </c>
       <c r="E27" t="str">
-        <f>C27&amp;"_"&amp;D27&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>1_12.jpeg</v>
       </c>
       <c r="F27" t="s">
@@ -5558,7 +5540,7 @@
         <v>68</v>
       </c>
       <c r="H27">
-        <f>C27</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I27" t="s">
@@ -5568,27 +5550,18 @@
         <v>52</v>
       </c>
       <c r="K27" t="str">
-        <f>F27</f>
+        <f t="shared" si="3"/>
         <v>Starry light bulb</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M27" t="s">
-        <v>63</v>
-      </c>
-      <c r="N27" t="str">
-        <f>G27</f>
-        <v>'</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="O27" s="3"/>
       <c r="P27" t="s">
         <v>64</v>
       </c>
       <c r="Q27">
-        <f>H27</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R27" t="s">
@@ -5598,7 +5571,7 @@
         <v>55</v>
       </c>
       <c r="U27" t="str">
-        <f>E27</f>
+        <f t="shared" si="6"/>
         <v>1_12.jpeg</v>
       </c>
       <c r="V27" s="3" t="s">
@@ -5608,7 +5581,7 @@
         <v>56</v>
       </c>
       <c r="X27" t="str">
-        <f>E27</f>
+        <f t="shared" si="7"/>
         <v>1_12.jpeg</v>
       </c>
       <c r="Y27" s="3" t="s">
@@ -5618,14 +5591,14 @@
         <v>60</v>
       </c>
       <c r="AC27" t="str">
-        <f>I27&amp;J27&amp;K27&amp;L27&amp;M27&amp;N27&amp;O27&amp;P27&amp;Q27&amp;R27&amp;S27&amp;T27&amp;U27&amp;V27&amp;W27&amp;X27&amp;Y27&amp;Z27&amp;AA27</f>
-        <v>a = Post.new({caption: 'Starry light bulb', location: ''', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_12.jpeg'), filename: '1_12.jpeg')a.save!</v>
+        <f t="shared" si="8"/>
+        <v>a = Post.new({caption: 'Starry light bulb', author_id: 1})a.photo.attach(io: File.open('app/assets/images/seed_images/1_12.jpeg'), filename: '1_12.jpeg')a.save!</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>74</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -5637,7 +5610,7 @@
         <v>2</v>
       </c>
       <c r="E28" t="str">
-        <f>C28&amp;"_"&amp;D28&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>3_2.jpeg</v>
       </c>
       <c r="F28" t="s">
@@ -5647,7 +5620,7 @@
         <v>68</v>
       </c>
       <c r="H28">
-        <f>C28</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I28" t="s">
@@ -5657,27 +5630,18 @@
         <v>52</v>
       </c>
       <c r="K28" t="str">
-        <f>F28</f>
+        <f t="shared" si="3"/>
         <v>Merry Christmas</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M28" t="s">
-        <v>63</v>
-      </c>
-      <c r="N28" t="str">
-        <f>G28</f>
-        <v>'</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="O28" s="3"/>
       <c r="P28" t="s">
         <v>64</v>
       </c>
       <c r="Q28">
-        <f>H28</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="R28" t="s">
@@ -5687,7 +5651,7 @@
         <v>55</v>
       </c>
       <c r="U28" t="str">
-        <f>E28</f>
+        <f t="shared" si="6"/>
         <v>3_2.jpeg</v>
       </c>
       <c r="V28" s="3" t="s">
@@ -5697,7 +5661,7 @@
         <v>56</v>
       </c>
       <c r="X28" t="str">
-        <f>E28</f>
+        <f t="shared" si="7"/>
         <v>3_2.jpeg</v>
       </c>
       <c r="Y28" s="3" t="s">
@@ -5707,14 +5671,14 @@
         <v>60</v>
       </c>
       <c r="AC28" t="str">
-        <f>I28&amp;J28&amp;K28&amp;L28&amp;M28&amp;N28&amp;O28&amp;P28&amp;Q28&amp;R28&amp;S28&amp;T28&amp;U28&amp;V28&amp;W28&amp;X28&amp;Y28&amp;Z28&amp;AA28</f>
-        <v>a = Post.new({caption: 'Merry Christmas', location: ''', author_id: 3})a.photo.attach(io: File.open('app/assets/images/seed_images/3_2.jpeg'), filename: '3_2.jpeg')a.save!</v>
+        <f t="shared" si="8"/>
+        <v>a = Post.new({caption: 'Merry Christmas', author_id: 3})a.photo.attach(io: File.open('app/assets/images/seed_images/3_2.jpeg'), filename: '3_2.jpeg')a.save!</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>98</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -5726,7 +5690,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="str">
-        <f>C29&amp;"_"&amp;D29&amp;".jpeg"</f>
+        <f t="shared" si="1"/>
         <v>5_2.jpeg</v>
       </c>
       <c r="F29" t="s">
@@ -5736,7 +5700,7 @@
         <v>15</v>
       </c>
       <c r="H29">
-        <f>C29</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I29" t="s">
@@ -5746,7 +5710,7 @@
         <v>52</v>
       </c>
       <c r="K29" t="str">
-        <f>F29</f>
+        <f t="shared" si="3"/>
         <v>Graffiti Boston</v>
       </c>
       <c r="L29" s="3" t="s">
@@ -5756,7 +5720,7 @@
         <v>63</v>
       </c>
       <c r="N29" t="str">
-        <f>G29</f>
+        <f t="shared" si="4"/>
         <v>Boston, MA</v>
       </c>
       <c r="O29" s="3" t="s">
@@ -5766,7 +5730,7 @@
         <v>64</v>
       </c>
       <c r="Q29">
-        <f>H29</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="R29" t="s">
@@ -5776,7 +5740,7 @@
         <v>55</v>
       </c>
       <c r="U29" t="str">
-        <f>E29</f>
+        <f t="shared" si="6"/>
         <v>5_2.jpeg</v>
       </c>
       <c r="V29" s="3" t="s">
@@ -5786,7 +5750,7 @@
         <v>56</v>
       </c>
       <c r="X29" t="str">
-        <f>E29</f>
+        <f t="shared" si="7"/>
         <v>5_2.jpeg</v>
       </c>
       <c r="Y29" s="3" t="s">
@@ -5796,7 +5760,7 @@
         <v>60</v>
       </c>
       <c r="AC29" t="str">
-        <f>I29&amp;J29&amp;K29&amp;L29&amp;M29&amp;N29&amp;O29&amp;P29&amp;Q29&amp;R29&amp;S29&amp;T29&amp;U29&amp;V29&amp;W29&amp;X29&amp;Y29&amp;Z29&amp;AA29</f>
+        <f t="shared" si="8"/>
         <v>a = Post.new({caption: 'Graffiti Boston', location: 'Boston, MA', author_id: 5})a.photo.attach(io: File.open('app/assets/images/seed_images/5_2.jpeg'), filename: '5_2.jpeg')a.save!</v>
       </c>
     </row>
@@ -5861,8 +5825,8 @@
         <v>54</v>
       </c>
       <c r="I4">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <f t="shared" ref="I4:I36" ca="1" si="0">RANDBETWEEN(1,5)</f>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
         <v>53</v>
@@ -5882,7 +5846,7 @@
       </c>
       <c r="O4" t="str">
         <f ca="1">A4&amp;B4&amp;C4&amp;D4&amp;E4&amp;F4&amp;G4&amp;H4&amp;I4&amp;J4&amp;K4&amp;L4&amp;M4</f>
-        <v>Comment.create!({post_id: 1, parent_comment_id: , author_id: 4, comment: 'That lighthouse!'})</v>
+        <v>Comment.create!({post_id: 1, parent_comment_id: , author_id: 3, comment: 'That lighthouse!'})</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -5908,8 +5872,8 @@
         <v>54</v>
       </c>
       <c r="I5">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="J5" t="s">
         <v>53</v>
@@ -5928,8 +5892,8 @@
         <v>Boomer staring into the flames</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" ref="O5:O36" ca="1" si="0">A5&amp;B5&amp;C5&amp;D5&amp;E5&amp;F5&amp;G5&amp;H5&amp;I5&amp;J5&amp;K5&amp;L5&amp;M5</f>
-        <v>Comment.create!({post_id: 2, parent_comment_id: , author_id: 3, comment: 'Cute doggie'})</v>
+        <f t="shared" ref="O5:O36" ca="1" si="1">A5&amp;B5&amp;C5&amp;D5&amp;E5&amp;F5&amp;G5&amp;H5&amp;I5&amp;J5&amp;K5&amp;L5&amp;M5</f>
+        <v>Comment.create!({post_id: 2, parent_comment_id: , author_id: 4, comment: 'Cute doggie'})</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -5955,8 +5919,8 @@
         <v>54</v>
       </c>
       <c r="I6">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J6" t="s">
         <v>53</v>
@@ -5975,8 +5939,8 @@
         <v>Arches</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 4, parent_comment_id: , author_id: 3, comment: 'Wow, that arch is huge!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 4, parent_comment_id: , author_id: 1, comment: 'Wow, that arch is huge!'})</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -6002,8 +5966,8 @@
         <v>54</v>
       </c>
       <c r="I7">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
         <v>53</v>
@@ -6022,8 +5986,8 @@
         <v>Arches</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 4, parent_comment_id: , author_id: 4, comment: 'Nice blue skies!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 4, parent_comment_id: , author_id: 3, comment: 'Nice blue skies!'})</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -6049,8 +6013,8 @@
         <v>54</v>
       </c>
       <c r="I8">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="J8" t="s">
         <v>53</v>
@@ -6069,8 +6033,8 @@
         <v>Snowy Firebird jump</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 5, parent_comment_id: , author_id: 2, comment: 'Omg! That jump in the snow!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 5, parent_comment_id: , author_id: 3, comment: 'Omg! That jump in the snow!'})</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -6096,8 +6060,8 @@
         <v>54</v>
       </c>
       <c r="I9">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="J9" t="s">
         <v>53</v>
@@ -6116,8 +6080,8 @@
         <v>SF Golden Gate Bridge 🌉</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 6, parent_comment_id: , author_id: 3, comment: 'Magestic!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 6, parent_comment_id: , author_id: 4, comment: 'Magestic!'})</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -6143,8 +6107,8 @@
         <v>54</v>
       </c>
       <c r="I10">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="J10" t="s">
         <v>53</v>
@@ -6163,8 +6127,8 @@
         <v>SF Golden Gate Bridge 🌉</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 6, parent_comment_id: , author_id: 5, comment: 'Great shot!!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 6, parent_comment_id: , author_id: 4, comment: 'Great shot!!'})</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -6190,8 +6154,8 @@
         <v>54</v>
       </c>
       <c r="I11">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
         <v>53</v>
@@ -6210,8 +6174,8 @@
         <v>Boston Night from above</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 8, parent_comment_id: , author_id: 5, comment: 'Wow, look at those light streaks'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 8, parent_comment_id: , author_id: 3, comment: 'Wow, look at those light streaks'})</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -6237,8 +6201,8 @@
         <v>54</v>
       </c>
       <c r="I12">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="J12" t="s">
         <v>53</v>
@@ -6257,8 +6221,8 @@
         <v>B&lt;3ston</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 10, parent_comment_id: , author_id: 3, comment: '&lt;3 Boston'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 10, parent_comment_id: , author_id: 5, comment: '&lt;3 Boston'})</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -6284,7 +6248,7 @@
         <v>54</v>
       </c>
       <c r="I13">
-        <f ca="1">RANDBETWEEN(1,5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="J13" t="s">
@@ -6304,7 +6268,7 @@
         <v>Peek-a-Boston</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>Comment.create!({post_id: 11, parent_comment_id: , author_id: 3, comment: 'Ooooo Boston'})</v>
       </c>
     </row>
@@ -6331,8 +6295,8 @@
         <v>54</v>
       </c>
       <c r="I14">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="J14" t="s">
         <v>53</v>
@@ -6351,8 +6315,8 @@
         <v>Make way for the Ducklings</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 12, parent_comment_id: , author_id: 4, comment: 'Quack quack'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 12, parent_comment_id: , author_id: 5, comment: 'Quack quack'})</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -6378,8 +6342,8 @@
         <v>54</v>
       </c>
       <c r="I15">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="J15" t="s">
         <v>53</v>
@@ -6398,8 +6362,8 @@
         <v>The U Bend.</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 14, parent_comment_id: , author_id: 4, comment: 'Horseshoeeeee'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 14, parent_comment_id: , author_id: 3, comment: 'Horseshoeeeee'})</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -6425,8 +6389,8 @@
         <v>54</v>
       </c>
       <c r="I16">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
       <c r="J16" t="s">
         <v>53</v>
@@ -6445,8 +6409,8 @@
         <v>Boston Sails by the Charles</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 15, parent_comment_id: , author_id: 5, comment: 'Great shot!!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 15, parent_comment_id: , author_id: 2, comment: 'Great shot!!'})</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -6472,8 +6436,8 @@
         <v>54</v>
       </c>
       <c r="I17">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="J17" t="s">
         <v>53</v>
@@ -6492,8 +6456,8 @@
         <v>Boston Sails by the Charles</v>
       </c>
       <c r="O17" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 15, parent_comment_id: , author_id: 5, comment: 'Wow!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 15, parent_comment_id: , author_id: 4, comment: 'Wow!'})</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -6519,8 +6483,8 @@
         <v>54</v>
       </c>
       <c r="I18">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="J18" t="s">
         <v>53</v>
@@ -6539,8 +6503,8 @@
         <v>Swinging away</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 16, parent_comment_id: , author_id: 1, comment: 'Weeeeeeee'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 16, parent_comment_id: , author_id: 3, comment: 'Weeeeeeee'})</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -6566,8 +6530,8 @@
         <v>54</v>
       </c>
       <c r="I19">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J19" t="s">
         <v>53</v>
@@ -6586,8 +6550,8 @@
         <v>Weeeeee</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 17, parent_comment_id: , author_id: 4, comment: '&lt;3 &lt;3'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 17, parent_comment_id: , author_id: 1, comment: '&lt;3 &lt;3'})</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -6613,8 +6577,8 @@
         <v>54</v>
       </c>
       <c r="I20">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="J20" t="s">
         <v>53</v>
@@ -6633,8 +6597,8 @@
         <v>Hidden path</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 18, parent_comment_id: , author_id: 2, comment: 'Wow, where is this?'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 18, parent_comment_id: , author_id: 5, comment: 'Wow, where is this?'})</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -6660,8 +6624,8 @@
         <v>54</v>
       </c>
       <c r="I21">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="J21" t="s">
         <v>53</v>
@@ -6680,8 +6644,8 @@
         <v>Boston from BU</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 19, parent_comment_id: , author_id: 4, comment: 'Awesome shot!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 19, parent_comment_id: , author_id: 5, comment: 'Awesome shot!'})</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -6707,7 +6671,7 @@
         <v>54</v>
       </c>
       <c r="I22">
-        <f ca="1">RANDBETWEEN(1,5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="J22" t="s">
@@ -6727,7 +6691,7 @@
         <v>Vivid coastal village</v>
       </c>
       <c r="O22" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>Comment.create!({post_id: 20, parent_comment_id: , author_id: 3, comment: 'Those colors are unreal!'})</v>
       </c>
     </row>
@@ -6754,8 +6718,8 @@
         <v>54</v>
       </c>
       <c r="I23">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J23" t="s">
         <v>53</v>
@@ -6774,8 +6738,8 @@
         <v>Vivid coastal village</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 20, parent_comment_id: , author_id: 2, comment: 'Wow!!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 20, parent_comment_id: , author_id: 1, comment: 'Wow!!'})</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -6801,8 +6765,8 @@
         <v>54</v>
       </c>
       <c r="I24">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="J24" t="s">
         <v>53</v>
@@ -6821,8 +6785,8 @@
         <v>iAmsterdam</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 21, parent_comment_id: , author_id: 2, comment: 'Amsterdam :D'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 21, parent_comment_id: , author_id: 3, comment: 'Amsterdam :D'})</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -6848,8 +6812,8 @@
         <v>54</v>
       </c>
       <c r="I25">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J25" t="s">
         <v>53</v>
@@ -6868,8 +6832,8 @@
         <v>Zion Overlook</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 22, parent_comment_id: , author_id: 4, comment: 'Nice shot!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 22, parent_comment_id: , author_id: 1, comment: 'Nice shot!'})</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -6895,8 +6859,8 @@
         <v>54</v>
       </c>
       <c r="I26">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J26" t="s">
         <v>53</v>
@@ -6915,8 +6879,8 @@
         <v>Zion Overlook</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 22, parent_comment_id: , author_id: 3, comment: 'Woahhh'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 22, parent_comment_id: , author_id: 1, comment: 'Woahhh'})</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -6942,8 +6906,8 @@
         <v>54</v>
       </c>
       <c r="I27">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="J27" t="s">
         <v>53</v>
@@ -6962,8 +6926,8 @@
         <v>Zion Overlook</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 22, parent_comment_id: , author_id: 2, comment: 'That is awesome!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 22, parent_comment_id: , author_id: 5, comment: 'That is awesome!'})</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -6989,8 +6953,8 @@
         <v>54</v>
       </c>
       <c r="I28">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J28" t="s">
         <v>53</v>
@@ -7009,8 +6973,8 @@
         <v>Bottle from Amsterdam</v>
       </c>
       <c r="O28" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 23, parent_comment_id: , author_id: 2, comment: 'Gulp gulp'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 23, parent_comment_id: , author_id: 1, comment: 'Gulp gulp'})</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -7036,8 +7000,8 @@
         <v>54</v>
       </c>
       <c r="I29">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J29" t="s">
         <v>53</v>
@@ -7056,8 +7020,8 @@
         <v>Boston from Longsfellow</v>
       </c>
       <c r="O29" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 24, parent_comment_id: , author_id: 2, comment: 'Wow, another great shot!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 24, parent_comment_id: , author_id: 1, comment: 'Wow, another great shot!'})</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -7083,8 +7047,8 @@
         <v>54</v>
       </c>
       <c r="I30">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
       <c r="J30" t="s">
         <v>53</v>
@@ -7103,8 +7067,8 @@
         <v>Boston from Longsfellow</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 24, parent_comment_id: , author_id: 5, comment: 'Great post!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 24, parent_comment_id: , author_id: 2, comment: 'Great post!'})</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -7130,7 +7094,7 @@
         <v>54</v>
       </c>
       <c r="I31">
-        <f ca="1">RANDBETWEEN(1,5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="J31" t="s">
@@ -7150,7 +7114,7 @@
         <v>Lets pool</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>Comment.create!({post_id: 25, parent_comment_id: , author_id: 3, comment: 'Lets play!'})</v>
       </c>
     </row>
@@ -7177,8 +7141,8 @@
         <v>54</v>
       </c>
       <c r="I32">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
         <v>53</v>
@@ -7197,8 +7161,8 @@
         <v>Lets pool</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 25, parent_comment_id: , author_id: 5, comment: '8-ball'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 25, parent_comment_id: , author_id: 1, comment: '8-ball'})</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -7224,7 +7188,7 @@
         <v>54</v>
       </c>
       <c r="I33">
-        <f ca="1">RANDBETWEEN(1,5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="J33" t="s">
@@ -7244,7 +7208,7 @@
         <v>Starry light bulb</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>Comment.create!({post_id: 26, parent_comment_id: , author_id: 3, comment: '💡 💡 💡 '})</v>
       </c>
     </row>
@@ -7271,8 +7235,8 @@
         <v>54</v>
       </c>
       <c r="I34">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="J34" t="s">
         <v>53</v>
@@ -7291,8 +7255,8 @@
         <v>Starry light bulb</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 26, parent_comment_id: , author_id: 3, comment: 'Nice bokeh!!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 26, parent_comment_id: , author_id: 5, comment: 'Nice bokeh!!'})</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -7318,8 +7282,8 @@
         <v>54</v>
       </c>
       <c r="I35">
-        <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="J35" t="s">
         <v>53</v>
@@ -7338,8 +7302,8 @@
         <v>Merry Christmas</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Comment.create!({post_id: 27, parent_comment_id: , author_id: 2, comment: 'Merry xmas!'})</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>Comment.create!({post_id: 27, parent_comment_id: , author_id: 3, comment: 'Merry xmas!'})</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -7365,7 +7329,7 @@
         <v>54</v>
       </c>
       <c r="I36">
-        <f ca="1">RANDBETWEEN(1,5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="J36" t="s">
@@ -7385,7 +7349,7 @@
         <v>Graffiti Boston</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>Comment.create!({post_id: 28, parent_comment_id: , author_id: 2, comment: 'Woah, where is this?'})</v>
       </c>
     </row>

</xml_diff>